<commit_message>
Update Import Student Template.xlsx
</commit_message>
<xml_diff>
--- a/System Information/Import Student Template.xlsx
+++ b/System Information/Import Student Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\Sams\System Information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Sams\System Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0195E2BC-EDCF-400A-BF89-D7698005BC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54EFCE9-2616-451D-ACDF-CF1D03641AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,10 +701,10 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="8" customWidth="1"/>
     <col min="2" max="2" width="41.42578125" style="1" customWidth="1"/>
@@ -716,7 +716,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="16.5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -739,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="4">
         <v>136612345678</v>
       </c>
@@ -768,7 +768,7 @@
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="4">
         <v>136618070392</v>
       </c>
@@ -795,7 +795,7 @@
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="4">
         <v>136656190043</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="4">
         <v>136622345678</v>
       </c>
@@ -849,7 +849,7 @@
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="16.5">
       <c r="A6" s="4">
         <v>136632345677</v>
       </c>
@@ -872,7 +872,7 @@
         <v>9256413897</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="16.5" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -887,7 +887,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="4"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -900,7 +900,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="4"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -913,7 +913,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="16.5">
       <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -926,7 +926,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -941,7 +941,7 @@
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -954,7 +954,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -967,7 +967,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -976,7 +976,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="4"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -991,7 +991,7 @@
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1004,7 +1004,7 @@
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1017,7 +1017,7 @@
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="4"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1026,7 +1026,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="16.5" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1041,7 +1041,7 @@
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="4"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1054,7 +1054,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="4"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1067,7 +1067,7 @@
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="4"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1080,7 +1080,7 @@
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="4"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1089,7 +1089,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="4"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1104,7 +1104,7 @@
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="4"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1117,7 +1117,7 @@
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="4"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1130,7 +1130,7 @@
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="4"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1139,7 +1139,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="4"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1154,7 +1154,7 @@
       <c r="K28" s="11"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1167,7 +1167,7 @@
       <c r="K29" s="14"/>
       <c r="L29" s="15"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="4"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1180,7 +1180,7 @@
       <c r="K30" s="14"/>
       <c r="L30" s="15"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="4"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1193,7 +1193,7 @@
       <c r="K31" s="17"/>
       <c r="L31" s="18"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="4"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1202,7 +1202,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="16.5" customHeight="1">
       <c r="A33" s="4"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1217,7 +1217,7 @@
       <c r="K33" s="19"/>
       <c r="L33" s="19"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="4"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1230,7 +1230,7 @@
       <c r="K34" s="19"/>
       <c r="L34" s="19"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="4"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1243,7 +1243,7 @@
       <c r="K35" s="19"/>
       <c r="L35" s="19"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="4"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1256,7 +1256,7 @@
       <c r="K36" s="19"/>
       <c r="L36" s="19"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="4"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1269,7 +1269,7 @@
       <c r="K37" s="19"/>
       <c r="L37" s="19"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="4"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1282,7 +1282,7 @@
       <c r="K38" s="19"/>
       <c r="L38" s="19"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="4"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1291,7 +1291,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="4"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1300,7 +1300,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="4"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1309,7 +1309,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="4"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1318,7 +1318,7 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="4"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1327,7 +1327,7 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" s="4"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1336,7 +1336,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" s="4"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1345,7 +1345,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46" s="4"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1354,7 +1354,7 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47" s="4"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1363,7 +1363,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" s="4"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1372,7 +1372,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1381,7 +1381,7 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="4"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1390,7 +1390,7 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" s="4"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1399,7 +1399,7 @@
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" s="4"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>

</xml_diff>